<commit_message>
kelas eksport import excel and database relational
</commit_message>
<xml_diff>
--- a/public/template/template_siswa.xlsx
+++ b/public/template/template_siswa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>no</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>gender (isikan L/P)</t>
+  </si>
+  <si>
+    <t>Kelas</t>
   </si>
 </sst>
 </file>
@@ -362,9 +365,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -372,7 +377,7 @@
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -385,6 +390,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upload siswa : add nisn
</commit_message>
<xml_diff>
--- a/public/template/template_siswa.xlsx
+++ b/public/template/template_siswa.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project\mtsn1tegal\mtsn-1-tegal-app\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\mtsn-1-tegal-app\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188035FF-A7B3-41F4-8800-E6CE6B33F65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>no</t>
   </si>
@@ -39,12 +40,15 @@
   </si>
   <si>
     <t>Kelas</t>
+  </si>
+  <si>
+    <t>nisn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,20 +368,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -385,12 +389,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>